<commit_message>
Files updated, more reference images
</commit_message>
<xml_diff>
--- a/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
+++ b/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="132">
   <si>
     <t>ARMORS</t>
   </si>
@@ -93,36 +93,6 @@
     <t>RARITY</t>
   </si>
   <si>
-    <t>Yokudan Heavy Helm</t>
-  </si>
-  <si>
-    <t>Yokudan Heavy Cuirass</t>
-  </si>
-  <si>
-    <t>Yokudan Heavy Gauntlets</t>
-  </si>
-  <si>
-    <t>Yokudan Heavy Boots</t>
-  </si>
-  <si>
-    <t>Yokudan Heavy Shield</t>
-  </si>
-  <si>
-    <t>Yokudan Light Helm</t>
-  </si>
-  <si>
-    <t>Yokudan Light Cuirass</t>
-  </si>
-  <si>
-    <t>Yokudan Light Gloves</t>
-  </si>
-  <si>
-    <t>Yokudan Light Boots</t>
-  </si>
-  <si>
-    <t>Yokudan Light Shield</t>
-  </si>
-  <si>
     <t>Dwemer Resin Helm</t>
   </si>
   <si>
@@ -427,6 +397,69 @@
   </si>
   <si>
     <t>Psijic Mystical Aegis</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Helm</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Plate</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Gauntlets</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Boots</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Aegis</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Helm</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Crown</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Mail</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Gloves</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Footwear</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Regalia</t>
+  </si>
+  <si>
+    <t>Aedric Heavenly Buckler</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Plate</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Gauntlets</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Boots</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Aegis</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Headgear</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Mail</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Gloves</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Footwear</t>
+  </si>
+  <si>
+    <t>Yokudan Ansei Buckler</t>
   </si>
 </sst>
 </file>
@@ -846,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L134"/>
+  <dimension ref="B1:L145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D111" sqref="D111"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,992 +949,1080 @@
         <v>8</v>
       </c>
       <c r="J8" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="C10" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>11</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>12</v>
+        <v>125</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>13</v>
+        <v>126</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>14</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>15</v>
+        <v>128</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>16</v>
+        <v>129</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>17</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>18</v>
+        <v>131</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C39" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="C40" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C42" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C43" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C44" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C45" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C46" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="C49" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="C50" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C51" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C52" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="C53" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="C54" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C55" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C56" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C57" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C58" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C59" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="C61" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="C62" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C63" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C64" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="C65" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C66" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="C67" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="C68" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C69" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="C70" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="C71" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="C73" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C74" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C75" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C76" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C77" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C78" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C79" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C80" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C81" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C82" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C83" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="C84" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C85" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C86" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C87" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C88" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C89" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C90" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C91" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C92" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C97" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C98" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C99" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C100" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C101" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C102" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C103" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C104" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C105" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="C106" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C112" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C113" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C114" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C115" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C116" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C117" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C118" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C119" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C120" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C121" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="C122" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="C123" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="C124" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="C125" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C126" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="C127" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="C128" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="C129" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="C130" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="C131" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="C132" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C133" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="C134" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>111</v>
+      </c>
+      <c r="C135" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>112</v>
+      </c>
+      <c r="C136" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>113</v>
+      </c>
+      <c r="C137" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>114</v>
+      </c>
+      <c r="C138" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>115</v>
+      </c>
+      <c r="C139" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>117</v>
+      </c>
+      <c r="C140" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>118</v>
+      </c>
+      <c r="C141" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>119</v>
+      </c>
+      <c r="C142" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>120</v>
+      </c>
+      <c r="C143" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>122</v>
+      </c>
+      <c r="C144" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>121</v>
+      </c>
+      <c r="C145" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adamantium armor references added
</commit_message>
<xml_diff>
--- a/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
+++ b/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="127">
   <si>
     <t>ARMORS</t>
   </si>
@@ -144,33 +144,6 @@
     <t>BONUS(ES)</t>
   </si>
   <si>
-    <t>Ra Gada Heavy Cuirass</t>
-  </si>
-  <si>
-    <t>Ra Gada Heavy Gauntlets</t>
-  </si>
-  <si>
-    <t>Ra Gada Heavy Helm</t>
-  </si>
-  <si>
-    <t>Ra Gada Heavy Boots</t>
-  </si>
-  <si>
-    <t>Ra Gada Heavy Shield</t>
-  </si>
-  <si>
-    <t>Ra Gada Light Helm</t>
-  </si>
-  <si>
-    <t>Ra Gada Light Cuirass</t>
-  </si>
-  <si>
-    <t>Ra Gada Light Boots</t>
-  </si>
-  <si>
-    <t>Ra Gada Light Shield</t>
-  </si>
-  <si>
     <t>Dwemer Adamant Helm</t>
   </si>
   <si>
@@ -342,9 +315,6 @@
     <t>Dwemer Adamant Gauntlets</t>
   </si>
   <si>
-    <t>Ra Gada Light Gloves</t>
-  </si>
-  <si>
     <t>Light Headgear</t>
   </si>
   <si>
@@ -460,6 +430,21 @@
   </si>
   <si>
     <t>Yokudan Ansei Buckler</t>
+  </si>
+  <si>
+    <t>Nordic Trollbone Helm</t>
+  </si>
+  <si>
+    <t>Nordic Trollbone Cuirass</t>
+  </si>
+  <si>
+    <t>Nordic Trollbone Gauntlet</t>
+  </si>
+  <si>
+    <t>Nordic Trollbone Boots</t>
+  </si>
+  <si>
+    <t>Nordic Trollbone Shield</t>
   </si>
 </sst>
 </file>
@@ -879,10 +864,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L145"/>
+  <dimension ref="B1:L140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,83 +942,83 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="L12" s="1"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
@@ -1041,7 +1026,7 @@
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
@@ -1049,7 +1034,7 @@
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
@@ -1057,7 +1042,7 @@
         <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
@@ -1065,7 +1050,7 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
@@ -1073,7 +1058,7 @@
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
@@ -1081,7 +1066,7 @@
         <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
@@ -1089,7 +1074,7 @@
         <v>15</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
@@ -1097,7 +1082,7 @@
         <v>16</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
@@ -1105,7 +1090,7 @@
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="2:3" x14ac:dyDescent="0.25">
@@ -1113,7 +1098,7 @@
         <v>18</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
@@ -1121,7 +1106,7 @@
         <v>19</v>
       </c>
       <c r="C29" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
@@ -1129,7 +1114,7 @@
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
@@ -1137,7 +1122,7 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
@@ -1145,7 +1130,7 @@
         <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.25">
@@ -1153,167 +1138,167 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C35" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>27</v>
+        <v>82</v>
       </c>
       <c r="C36" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C39" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="C41" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
         <v>33</v>
-      </c>
-      <c r="C42" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
         <v>34</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>35</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>36</v>
+        <v>87</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>37</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>38</v>
+        <v>91</v>
       </c>
       <c r="C48" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="C49" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="C50" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="C51" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="C53" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
@@ -1326,138 +1311,138 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>97</v>
+        <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="C56" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="C57" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>101</v>
+        <v>48</v>
       </c>
       <c r="C58" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>103</v>
+        <v>50</v>
       </c>
       <c r="C60" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="C61" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>105</v>
+        <v>52</v>
       </c>
       <c r="C62" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>107</v>
+        <v>53</v>
       </c>
       <c r="C63" t="s">
-        <v>106</v>
+        <v>30</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>108</v>
+        <v>54</v>
       </c>
       <c r="C64" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C65" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C66" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C67" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C68" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C69" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C70" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C71" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
@@ -1465,332 +1450,332 @@
         <v>61</v>
       </c>
       <c r="C72" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C73" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C74" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C75" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C76" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C77" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C78" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C79" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C80" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C81" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C82" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>70</v>
-      </c>
-      <c r="C83" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>70</v>
-      </c>
-      <c r="C84" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>71</v>
-      </c>
-      <c r="C85" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>71</v>
-      </c>
-      <c r="C86" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C87" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>71</v>
+        <v>99</v>
       </c>
       <c r="C88" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="C89" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>73</v>
+        <v>99</v>
       </c>
       <c r="C90" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="C91" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C92" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="C93" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="C94" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="C95" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="C96" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>109</v>
-      </c>
-      <c r="C97" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>109</v>
-      </c>
-      <c r="C98" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>109</v>
-      </c>
-      <c r="C99" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>109</v>
-      </c>
-      <c r="C100" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>110</v>
-      </c>
-      <c r="C101" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C102" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C103" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C104" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C105" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C106" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C107" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C108" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C109" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C110" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>75</v>
+        <v>68</v>
+      </c>
+      <c r="C111" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C112" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C113" t="s">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C114" t="s">
-        <v>41</v>
+        <v>85</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C115" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C116" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
@@ -1798,55 +1783,55 @@
         <v>77</v>
       </c>
       <c r="C117" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C118" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C119" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C120" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C121" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C122" t="s">
-        <v>93</v>
+        <v>36</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C123" t="s">
-        <v>94</v>
+        <v>37</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
@@ -1854,87 +1839,87 @@
         <v>81</v>
       </c>
       <c r="C124" t="s">
-        <v>95</v>
+        <v>38</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="C125" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="C126" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C127" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="C128" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
       <c r="C129" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="C130" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="C131" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>85</v>
+        <v>109</v>
       </c>
       <c r="C132" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>89</v>
+        <v>110</v>
       </c>
       <c r="C133" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>90</v>
+        <v>112</v>
       </c>
       <c r="C134" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
@@ -1942,87 +1927,47 @@
         <v>111</v>
       </c>
       <c r="C135" t="s">
-        <v>39</v>
+        <v>96</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>112</v>
+        <v>122</v>
       </c>
       <c r="C136" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="C137" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="C138" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C139" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="C140" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B141" t="s">
-        <v>118</v>
-      </c>
-      <c r="C141" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>119</v>
-      </c>
-      <c r="C142" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B143" t="s">
-        <v>120</v>
-      </c>
-      <c r="C143" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B144" t="s">
-        <v>122</v>
-      </c>
-      <c r="C144" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B145" t="s">
-        <v>121</v>
-      </c>
-      <c r="C145" t="s">
-        <v>106</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
I cant even track how much stuff i updated...
</commit_message>
<xml_diff>
--- a/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
+++ b/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9DEBDAE2-5BA9-4A21-A57F-04D351020284}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -450,7 +451,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -863,27 +864,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
-      <selection activeCell="E143" sqref="E143"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
@@ -896,7 +897,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -907,8 +908,8 @@
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="2:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -940,7 +941,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>106</v>
       </c>
@@ -948,7 +949,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>113</v>
       </c>
@@ -956,7 +957,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>114</v>
       </c>
@@ -964,7 +965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>115</v>
       </c>
@@ -973,7 +974,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>116</v>
       </c>
@@ -981,7 +982,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>117</v>
       </c>
@@ -989,7 +990,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>118</v>
       </c>
@@ -997,7 +998,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>119</v>
       </c>
@@ -1005,7 +1006,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>120</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>121</v>
       </c>
@@ -1021,7 +1022,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>9</v>
       </c>
@@ -1029,7 +1030,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -1037,7 +1038,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>12</v>
       </c>
@@ -1053,7 +1054,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -1061,7 +1062,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -1069,7 +1070,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>15</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>16</v>
       </c>
@@ -1085,7 +1086,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>17</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>18</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>19</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>20</v>
       </c>
@@ -1117,7 +1118,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>21</v>
       </c>
@@ -1125,7 +1126,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>22</v>
       </c>
@@ -1133,7 +1134,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>23</v>
       </c>
@@ -1141,7 +1142,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>26</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>27</v>
       </c>
@@ -1157,7 +1158,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>82</v>
       </c>
@@ -1165,7 +1166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>28</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>29</v>
       </c>
@@ -1181,7 +1182,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>40</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>41</v>
       </c>
@@ -1197,7 +1198,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>42</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>43</v>
       </c>
@@ -1213,7 +1214,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>44</v>
       </c>
@@ -1221,7 +1222,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>88</v>
       </c>
@@ -1229,7 +1230,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>87</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>89</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>90</v>
       </c>
@@ -1253,7 +1254,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>91</v>
       </c>
@@ -1261,7 +1262,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>92</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>93</v>
       </c>
@@ -1277,7 +1278,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>94</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>95</v>
       </c>
@@ -1293,7 +1294,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>97</v>
       </c>
@@ -1301,7 +1302,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>98</v>
       </c>
@@ -1309,7 +1310,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>45</v>
       </c>
@@ -1317,7 +1318,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>46</v>
       </c>
@@ -1325,7 +1326,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>47</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>48</v>
       </c>
@@ -1341,7 +1342,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>49</v>
       </c>
@@ -1349,7 +1350,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>50</v>
       </c>
@@ -1357,7 +1358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>51</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>52</v>
       </c>
@@ -1373,7 +1374,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>53</v>
       </c>
@@ -1381,7 +1382,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>54</v>
       </c>
@@ -1389,7 +1390,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>55</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>56</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>57</v>
       </c>
@@ -1413,7 +1414,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>58</v>
       </c>
@@ -1421,7 +1422,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>59</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>60</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>61</v>
       </c>
@@ -1445,7 +1446,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>61</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>61</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>61</v>
       </c>
@@ -1469,7 +1470,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>62</v>
       </c>
@@ -1477,7 +1478,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>62</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B77" t="s">
         <v>62</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>62</v>
       </c>
@@ -1501,7 +1502,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B79" t="s">
         <v>64</v>
       </c>
@@ -1509,7 +1510,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B80" t="s">
         <v>64</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
         <v>64</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B82" t="s">
         <v>64</v>
       </c>
@@ -1533,27 +1534,27 @@
         <v>38</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B85" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
         <v>99</v>
       </c>
@@ -1561,7 +1562,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
         <v>99</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B89" t="s">
         <v>99</v>
       </c>
@@ -1577,7 +1578,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
         <v>99</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>100</v>
       </c>
@@ -1593,7 +1594,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B92" t="s">
         <v>65</v>
       </c>
@@ -1601,7 +1602,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>65</v>
       </c>
@@ -1609,7 +1610,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B94" t="s">
         <v>65</v>
       </c>
@@ -1617,7 +1618,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B95" t="s">
         <v>65</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
         <v>65</v>
       </c>
@@ -1633,32 +1634,32 @@
         <v>39</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B98" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B99" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B101" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B102" t="s">
         <v>67</v>
       </c>
@@ -1666,7 +1667,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>67</v>
       </c>
@@ -1674,7 +1675,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B104" t="s">
         <v>67</v>
       </c>
@@ -1682,7 +1683,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>67</v>
       </c>
@@ -1690,7 +1691,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>67</v>
       </c>
@@ -1698,7 +1699,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>68</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>68</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B109" t="s">
         <v>68</v>
       </c>
@@ -1722,7 +1723,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
         <v>68</v>
       </c>
@@ -1730,7 +1731,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B111" t="s">
         <v>68</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B112" t="s">
         <v>69</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B113" t="s">
         <v>70</v>
       </c>
@@ -1754,7 +1755,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B114" t="s">
         <v>72</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B115" t="s">
         <v>71</v>
       </c>
@@ -1770,7 +1771,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B116" t="s">
         <v>75</v>
       </c>
@@ -1778,7 +1779,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B117" t="s">
         <v>77</v>
       </c>
@@ -1786,7 +1787,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
         <v>74</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>78</v>
       </c>
@@ -1802,7 +1803,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>73</v>
       </c>
@@ -1810,7 +1811,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B121" t="s">
         <v>79</v>
       </c>
@@ -1818,7 +1819,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B122" t="s">
         <v>76</v>
       </c>
@@ -1826,7 +1827,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B123" t="s">
         <v>80</v>
       </c>
@@ -1834,7 +1835,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B124" t="s">
         <v>81</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B125" t="s">
         <v>101</v>
       </c>
@@ -1850,7 +1851,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
         <v>102</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B127" t="s">
         <v>103</v>
       </c>
@@ -1866,7 +1867,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B128" t="s">
         <v>104</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B129" t="s">
         <v>105</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B130" t="s">
         <v>107</v>
       </c>
@@ -1890,7 +1891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B131" t="s">
         <v>108</v>
       </c>
@@ -1898,7 +1899,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B132" t="s">
         <v>109</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B133" t="s">
         <v>110</v>
       </c>
@@ -1914,7 +1915,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B134" t="s">
         <v>112</v>
       </c>
@@ -1922,7 +1923,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B135" t="s">
         <v>111</v>
       </c>
@@ -1930,7 +1931,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B136" t="s">
         <v>122</v>
       </c>
@@ -1938,7 +1939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B137" t="s">
         <v>123</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B138" t="s">
         <v>124</v>
       </c>
@@ -1954,7 +1955,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B139" t="s">
         <v>125</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B140" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
Exotic armors table updated
</commit_message>
<xml_diff>
--- a/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
+++ b/Files/Tables/Equipment/Exotic/Exotic Armors.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="175">
   <si>
     <t>ARMORS</t>
   </si>
@@ -201,30 +201,6 @@
     <t>Ancient Orc Shield</t>
   </si>
   <si>
-    <t>Dark Brotherhood Heavy Helm</t>
-  </si>
-  <si>
-    <t>Dark Brotherhood Heavy Cuirass</t>
-  </si>
-  <si>
-    <t>Dark Brotherhood Heavy Gauntlets</t>
-  </si>
-  <si>
-    <t>Dark Brotherhood Heavy Boots</t>
-  </si>
-  <si>
-    <t>Dark Brotherhood Light Helm</t>
-  </si>
-  <si>
-    <t>Dark Brotherhood Light Cuirass</t>
-  </si>
-  <si>
-    <t>Dark Brotherhood Light Gloves</t>
-  </si>
-  <si>
-    <t>Dark Brotherhood Light Boots</t>
-  </si>
-  <si>
     <t>Tsaesci Heavy Helm</t>
   </si>
   <si>
@@ -252,18 +228,9 @@
     <t>Khajiit Ceremonial</t>
   </si>
   <si>
-    <t>Argonian Tribal</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ancient Dragon </t>
   </si>
   <si>
-    <t>Thieves Guild Heavy</t>
-  </si>
-  <si>
-    <t>Thieves Guild Light</t>
-  </si>
-  <si>
     <t>Dibella priest Mask</t>
   </si>
   <si>
@@ -511,6 +478,117 @@
   </si>
   <si>
     <t>Argonian Leaf Footwear</t>
+  </si>
+  <si>
+    <t>Netch Leather Cap</t>
+  </si>
+  <si>
+    <t>Netch Leather Coat</t>
+  </si>
+  <si>
+    <t>Netch Leather Gloves</t>
+  </si>
+  <si>
+    <t>Netch Leather Boots</t>
+  </si>
+  <si>
+    <t>Netch Leather Buckler</t>
+  </si>
+  <si>
+    <t>Cyrodilic Mithril Helm</t>
+  </si>
+  <si>
+    <t>Cyrodilic Mithril Mail</t>
+  </si>
+  <si>
+    <t>Cyrodilic Mithril Gloves</t>
+  </si>
+  <si>
+    <t>Cyrodilic Mithril Boots</t>
+  </si>
+  <si>
+    <t>Cyrodilic Mithril Shield</t>
+  </si>
+  <si>
+    <t>Akaviri Dragonscale Helm</t>
+  </si>
+  <si>
+    <t>Akaviri Dragonscale Mail</t>
+  </si>
+  <si>
+    <t>Akaviri Dragonscale Gloves</t>
+  </si>
+  <si>
+    <t>Akaviri Dragonscale Boots</t>
+  </si>
+  <si>
+    <t>Akaviri Dragonscale Shield</t>
+  </si>
+  <si>
+    <t>Dark Brotherhood Enforcer Helm</t>
+  </si>
+  <si>
+    <t>Dark Brotherhood Enforcer Cuirass</t>
+  </si>
+  <si>
+    <t>Dark Brotherhood Enforcer Gauntlets</t>
+  </si>
+  <si>
+    <t>Dark Brotherhood Enforcer Boots</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Helm</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Mail</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Gloves</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Boots</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Shield</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Mask</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Tunic</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Footwear</t>
+  </si>
+  <si>
+    <t>Argonian Tribal Headdress</t>
+  </si>
+  <si>
+    <t>Argonian Tribal Garment</t>
+  </si>
+  <si>
+    <t>Argonian Tribal Hand Wraps</t>
+  </si>
+  <si>
+    <t>Ancient Ra Gada Hand Wraps</t>
+  </si>
+  <si>
+    <t>Argonian Tribal Foot Wraps</t>
+  </si>
+  <si>
+    <t>Argonian Leviathan Helm</t>
+  </si>
+  <si>
+    <t>Argonian Leviathan Gauntlets</t>
+  </si>
+  <si>
+    <t>Argonian Leviathan Boots</t>
+  </si>
+  <si>
+    <t>Argonian Leviathan Shield</t>
+  </si>
+  <si>
+    <t>Argonian Leviathan Mail</t>
   </si>
 </sst>
 </file>
@@ -930,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:L149"/>
+  <dimension ref="B1:L164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" workbookViewId="0">
-      <selection activeCell="D148" sqref="D148"/>
+    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
+      <selection activeCell="B165" sqref="B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1086,7 @@
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C9" t="s">
         <v>30</v>
@@ -1016,7 +1094,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
         <v>31</v>
@@ -1024,7 +1102,7 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -1032,7 +1110,7 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C12" t="s">
         <v>33</v>
@@ -1041,7 +1119,7 @@
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C13" t="s">
         <v>34</v>
@@ -1049,7 +1127,7 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -1057,7 +1135,7 @@
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C15" t="s">
         <v>36</v>
@@ -1065,7 +1143,7 @@
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
         <v>37</v>
@@ -1073,7 +1151,7 @@
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1081,7 +1159,7 @@
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="C18" t="s">
         <v>39</v>
@@ -1225,7 +1303,7 @@
     </row>
     <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="C36" t="s">
         <v>32</v>
@@ -1289,7 +1367,7 @@
     </row>
     <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
         <v>30</v>
@@ -1297,7 +1375,7 @@
     </row>
     <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C45" t="s">
         <v>31</v>
@@ -1305,7 +1383,7 @@
     </row>
     <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C46" t="s">
         <v>32</v>
@@ -1313,7 +1391,7 @@
     </row>
     <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C47" t="s">
         <v>33</v>
@@ -1321,7 +1399,7 @@
     </row>
     <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
       <c r="C48" t="s">
         <v>34</v>
@@ -1329,7 +1407,7 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="C49" t="s">
         <v>35</v>
@@ -1337,7 +1415,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="C50" t="s">
         <v>36</v>
@@ -1345,7 +1423,7 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="C51" t="s">
         <v>37</v>
@@ -1353,7 +1431,7 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C52" t="s">
         <v>38</v>
@@ -1361,15 +1439,15 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="C53" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="C54" t="s">
         <v>39</v>
@@ -1377,7 +1455,7 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>45</v>
+        <v>153</v>
       </c>
       <c r="C55" t="s">
         <v>30</v>
@@ -1385,7 +1463,7 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>46</v>
+        <v>154</v>
       </c>
       <c r="C56" t="s">
         <v>31</v>
@@ -1393,7 +1471,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>47</v>
+        <v>155</v>
       </c>
       <c r="C57" t="s">
         <v>32</v>
@@ -1401,7 +1479,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>48</v>
+        <v>156</v>
       </c>
       <c r="C58" t="s">
         <v>33</v>
@@ -1409,135 +1487,135 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C59" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C60" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C61" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C62" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C63" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C64" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C65" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C66" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="C67" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>58</v>
+        <v>106</v>
       </c>
       <c r="C68" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="C69" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="C70" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C71" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="C72" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C73" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C74" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>113</v>
+        <v>165</v>
       </c>
       <c r="C75" t="s">
         <v>35</v>
@@ -1545,7 +1623,7 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
-        <v>114</v>
+        <v>166</v>
       </c>
       <c r="C76" t="s">
         <v>36</v>
@@ -1553,7 +1631,7 @@
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
-        <v>120</v>
+        <v>167</v>
       </c>
       <c r="C77" t="s">
         <v>37</v>
@@ -1561,7 +1639,7 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>115</v>
+        <v>169</v>
       </c>
       <c r="C78" t="s">
         <v>38</v>
@@ -1569,164 +1647,164 @@
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
-        <v>62</v>
-      </c>
-      <c r="C79" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>62</v>
-      </c>
-      <c r="C80" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>62</v>
-      </c>
-      <c r="C81" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
-        <v>62</v>
-      </c>
-      <c r="C82" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
-        <v>61</v>
+        <v>120</v>
+      </c>
+      <c r="C83" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
-        <v>61</v>
+        <v>121</v>
+      </c>
+      <c r="C84" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
-        <v>61</v>
+        <v>122</v>
+      </c>
+      <c r="C85" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
-        <v>61</v>
+        <v>123</v>
+      </c>
+      <c r="C86" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C88" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C89" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="C91" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="C92" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>135</v>
-      </c>
-      <c r="C93" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>136</v>
-      </c>
-      <c r="C94" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>137</v>
-      </c>
-      <c r="C95" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>139</v>
-      </c>
-      <c r="C96" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>63</v>
+        <v>55</v>
+      </c>
+      <c r="C98" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>63</v>
+        <v>56</v>
+      </c>
+      <c r="C99" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="C100" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="C101" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C102" t="s">
         <v>30</v>
@@ -1734,7 +1812,7 @@
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C103" t="s">
         <v>31</v>
@@ -1742,7 +1820,7 @@
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C104" t="s">
         <v>32</v>
@@ -1758,7 +1836,7 @@
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C106" t="s">
         <v>34</v>
@@ -1774,7 +1852,7 @@
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C108" t="s">
         <v>36</v>
@@ -1782,7 +1860,7 @@
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C109" t="s">
         <v>37</v>
@@ -1790,7 +1868,7 @@
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C110" t="s">
         <v>38</v>
@@ -1798,314 +1876,347 @@
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="C111" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>66</v>
+        <v>87</v>
       </c>
       <c r="C112" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>67</v>
+        <v>88</v>
       </c>
       <c r="C113" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="C114" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
-        <v>68</v>
+        <v>90</v>
       </c>
       <c r="C115" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C116" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="C117" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
-        <v>71</v>
+        <v>93</v>
       </c>
       <c r="C118" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="C119" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="C120" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="C121" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="C122" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>77</v>
+        <v>98</v>
       </c>
       <c r="C123" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="C124" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C125" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C126" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="C127" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="C129" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>103</v>
+        <v>133</v>
       </c>
       <c r="C131" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
-        <v>104</v>
+        <v>134</v>
       </c>
       <c r="C132" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C133" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="C134" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="C135" t="s">
-        <v>93</v>
+        <v>38</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" t="s">
-        <v>108</v>
-      </c>
-      <c r="C136" t="s">
-        <v>30</v>
+        <v>138</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
-        <v>109</v>
-      </c>
-      <c r="C137" t="s">
-        <v>31</v>
+        <v>139</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" t="s">
-        <v>110</v>
-      </c>
-      <c r="C138" t="s">
-        <v>32</v>
+        <v>140</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
-        <v>111</v>
-      </c>
-      <c r="C139" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" t="s">
-        <v>112</v>
-      </c>
-      <c r="C140" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
-        <v>140</v>
-      </c>
-      <c r="C141" t="s">
-        <v>30</v>
+        <v>143</v>
       </c>
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" t="s">
-        <v>141</v>
-      </c>
-      <c r="C142" t="s">
-        <v>31</v>
+        <v>144</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" t="s">
-        <v>142</v>
-      </c>
-      <c r="C143" t="s">
-        <v>32</v>
+        <v>145</v>
       </c>
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>143</v>
-      </c>
-      <c r="C144" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>144</v>
-      </c>
-      <c r="C145" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>145</v>
-      </c>
-      <c r="C146" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>146</v>
-      </c>
-      <c r="C147" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>147</v>
-      </c>
-      <c r="C148" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>148</v>
-      </c>
-      <c r="C149" t="s">
-        <v>38</v>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B151" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B152" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B153" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B156" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B157" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B159" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B160" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B161" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B162" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B164" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>